<commit_message>
Add non defense buildings
</commit_message>
<xml_diff>
--- a/clash.xlsx
+++ b/clash.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="21075" windowHeight="8190" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="21075" windowHeight="8190" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Troops" sheetId="3" r:id="rId1"/>
     <sheet name="Defense" sheetId="4" r:id="rId2"/>
     <sheet name="Heros" sheetId="5" r:id="rId3"/>
+    <sheet name="Buildings" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
   <si>
     <t>housing</t>
   </si>
@@ -145,6 +146,63 @@
   </si>
   <si>
     <t>Giga Tesla</t>
+  </si>
+  <si>
+    <t>Town Hall</t>
+  </si>
+  <si>
+    <t>Gold Mine</t>
+  </si>
+  <si>
+    <t>Gold Storage</t>
+  </si>
+  <si>
+    <t>Elixir Collector</t>
+  </si>
+  <si>
+    <t>Elixir Storage</t>
+  </si>
+  <si>
+    <t>Dark Elixir Drill</t>
+  </si>
+  <si>
+    <t>Dark Elixir Storage</t>
+  </si>
+  <si>
+    <t>Clan Castle</t>
+  </si>
+  <si>
+    <t>Army Camp</t>
+  </si>
+  <si>
+    <t>Barracks</t>
+  </si>
+  <si>
+    <t>Dark Barracks</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
+  </si>
+  <si>
+    <t>Spell Factory</t>
+  </si>
+  <si>
+    <t>Dark Spell Factory</t>
+  </si>
+  <si>
+    <t>Workshop</t>
+  </si>
+  <si>
+    <t>BK Alter</t>
+  </si>
+  <si>
+    <t>AQ Alter</t>
+  </si>
+  <si>
+    <t>GW Alter</t>
+  </si>
+  <si>
+    <t>Builders Hut</t>
   </si>
 </sst>
 </file>
@@ -886,11 +944,12 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C1" sqref="C1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1071,7 +1130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1140,4 +1199,262 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30">
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>